<commit_message>
Randomly shuffle team names
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -22,91 +22,91 @@
     <t>Post 1</t>
   </si>
   <si>
+    <t>fys5</t>
+  </si>
+  <si>
+    <t>mat3</t>
+  </si>
+  <si>
+    <t>hold2</t>
+  </si>
+  <si>
+    <t>fys3</t>
+  </si>
+  <si>
+    <t>Post 2</t>
+  </si>
+  <si>
+    <t>dav</t>
+  </si>
+  <si>
+    <t>mat2</t>
+  </si>
+  <si>
+    <t>dat7</t>
+  </si>
+  <si>
+    <t>hold1</t>
+  </si>
+  <si>
+    <t>Post 3</t>
+  </si>
+  <si>
+    <t>fys4</t>
+  </si>
+  <si>
+    <t>fys2</t>
+  </si>
+  <si>
+    <t>møk1</t>
+  </si>
+  <si>
+    <t>it1</t>
+  </si>
+  <si>
+    <t>Post 4</t>
+  </si>
+  <si>
+    <t>nano</t>
+  </si>
+  <si>
+    <t>it2</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>mat1</t>
+  </si>
+  <si>
+    <t>Post 5</t>
+  </si>
+  <si>
+    <t>dat3</t>
+  </si>
+  <si>
+    <t>møk2</t>
+  </si>
+  <si>
+    <t>dat6</t>
+  </si>
+  <si>
+    <t>dat4</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>fys1</t>
+  </si>
+  <si>
     <t>dat1</t>
   </si>
   <si>
+    <t>dat5</t>
+  </si>
+  <si>
     <t>dat2</t>
-  </si>
-  <si>
-    <t>dat3</t>
-  </si>
-  <si>
-    <t>dat4</t>
-  </si>
-  <si>
-    <t>Post 2</t>
-  </si>
-  <si>
-    <t>dat5</t>
-  </si>
-  <si>
-    <t>dat6</t>
-  </si>
-  <si>
-    <t>dat7</t>
-  </si>
-  <si>
-    <t>dav</t>
-  </si>
-  <si>
-    <t>Post 3</t>
-  </si>
-  <si>
-    <t>fys1</t>
-  </si>
-  <si>
-    <t>fys2</t>
-  </si>
-  <si>
-    <t>fys3</t>
-  </si>
-  <si>
-    <t>fys4</t>
-  </si>
-  <si>
-    <t>Post 4</t>
-  </si>
-  <si>
-    <t>fys5</t>
-  </si>
-  <si>
-    <t>mat1</t>
-  </si>
-  <si>
-    <t>mat2</t>
-  </si>
-  <si>
-    <t>mat3</t>
-  </si>
-  <si>
-    <t>Post 5</t>
-  </si>
-  <si>
-    <t>møk1</t>
-  </si>
-  <si>
-    <t>møk2</t>
-  </si>
-  <si>
-    <t>nano</t>
-  </si>
-  <si>
-    <t>it1</t>
-  </si>
-  <si>
-    <t>Pause</t>
-  </si>
-  <si>
-    <t>it2</t>
-  </si>
-  <si>
-    <t>TK</t>
-  </si>
-  <si>
-    <t>hold1</t>
-  </si>
-  <si>
-    <t>hold2</t>
   </si>
   <si>
     <t>14:35-14:45</t>

</xml_diff>

<commit_message>
Improve speed of solving
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -22,91 +22,91 @@
     <t>Post 1</t>
   </si>
   <si>
+    <t>hold1</t>
+  </si>
+  <si>
+    <t>møk2</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
     <t>fys5</t>
   </si>
   <si>
+    <t>Post 2</t>
+  </si>
+  <si>
+    <t>fys4</t>
+  </si>
+  <si>
+    <t>hold2</t>
+  </si>
+  <si>
+    <t>dat5</t>
+  </si>
+  <si>
+    <t>fys2</t>
+  </si>
+  <si>
+    <t>Post 3</t>
+  </si>
+  <si>
+    <t>mat2</t>
+  </si>
+  <si>
+    <t>møk1</t>
+  </si>
+  <si>
+    <t>dat3</t>
+  </si>
+  <si>
+    <t>dat1</t>
+  </si>
+  <si>
+    <t>Post 4</t>
+  </si>
+  <si>
+    <t>dat6</t>
+  </si>
+  <si>
+    <t>dat7</t>
+  </si>
+  <si>
+    <t>dat4</t>
+  </si>
+  <si>
+    <t>fys1</t>
+  </si>
+  <si>
+    <t>Post 5</t>
+  </si>
+  <si>
+    <t>nano</t>
+  </si>
+  <si>
+    <t>dav</t>
+  </si>
+  <si>
     <t>mat3</t>
   </si>
   <si>
-    <t>hold2</t>
+    <t>it1</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>mat1</t>
+  </si>
+  <si>
+    <t>dat2</t>
+  </si>
+  <si>
+    <t>it2</t>
   </si>
   <si>
     <t>fys3</t>
-  </si>
-  <si>
-    <t>Post 2</t>
-  </si>
-  <si>
-    <t>dav</t>
-  </si>
-  <si>
-    <t>mat2</t>
-  </si>
-  <si>
-    <t>dat7</t>
-  </si>
-  <si>
-    <t>hold1</t>
-  </si>
-  <si>
-    <t>Post 3</t>
-  </si>
-  <si>
-    <t>fys4</t>
-  </si>
-  <si>
-    <t>fys2</t>
-  </si>
-  <si>
-    <t>møk1</t>
-  </si>
-  <si>
-    <t>it1</t>
-  </si>
-  <si>
-    <t>Post 4</t>
-  </si>
-  <si>
-    <t>nano</t>
-  </si>
-  <si>
-    <t>it2</t>
-  </si>
-  <si>
-    <t>TK</t>
-  </si>
-  <si>
-    <t>mat1</t>
-  </si>
-  <si>
-    <t>Post 5</t>
-  </si>
-  <si>
-    <t>dat3</t>
-  </si>
-  <si>
-    <t>møk2</t>
-  </si>
-  <si>
-    <t>dat6</t>
-  </si>
-  <si>
-    <t>dat4</t>
-  </si>
-  <si>
-    <t>Pause</t>
-  </si>
-  <si>
-    <t>fys1</t>
-  </si>
-  <si>
-    <t>dat1</t>
-  </si>
-  <si>
-    <t>dat5</t>
-  </si>
-  <si>
-    <t>dat2</t>
   </si>
   <si>
     <t>14:35-14:45</t>
@@ -620,16 +620,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -640,13 +640,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -654,16 +654,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -671,16 +671,16 @@
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -688,16 +688,16 @@
         <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -705,13 +705,13 @@
         <v>26</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>25</v>
@@ -731,13 +731,13 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>29</v>
@@ -748,16 +748,16 @@
         <v>6</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -768,10 +768,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>25</v>
@@ -782,16 +782,16 @@
         <v>16</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -799,16 +799,16 @@
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -816,13 +816,13 @@
         <v>26</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>24</v>
@@ -842,16 +842,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -859,16 +859,16 @@
         <v>6</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -876,16 +876,16 @@
         <v>11</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -896,13 +896,13 @@
         <v>2</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -910,16 +910,16 @@
         <v>21</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -927,16 +927,16 @@
         <v>26</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" customHeight="1">
@@ -953,13 +953,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>27</v>
@@ -970,16 +970,16 @@
         <v>6</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -987,16 +987,16 @@
         <v>11</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1007,13 +1007,13 @@
         <v>5</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1024,10 +1024,10 @@
         <v>2</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>30</v>
@@ -1038,16 +1038,16 @@
         <v>26</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" customHeight="1">
@@ -1064,16 +1064,16 @@
         <v>1</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1081,16 +1081,16 @@
         <v>6</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1098,16 +1098,16 @@
         <v>11</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1115,16 +1115,16 @@
         <v>16</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1132,13 +1132,13 @@
         <v>21</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>29</v>
@@ -1152,13 +1152,13 @@
         <v>2</v>
       </c>
       <c r="C52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="E52" s="3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sort team names on same activity
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -22,91 +22,91 @@
     <t>Post 1</t>
   </si>
   <si>
+    <t>dav</t>
+  </si>
+  <si>
+    <t>fys4</t>
+  </si>
+  <si>
+    <t>it2</t>
+  </si>
+  <si>
+    <t>mat2</t>
+  </si>
+  <si>
+    <t>Post 2</t>
+  </si>
+  <si>
+    <t>dat1</t>
+  </si>
+  <si>
+    <t>dat3</t>
+  </si>
+  <si>
+    <t>fys2</t>
+  </si>
+  <si>
+    <t>fys3</t>
+  </si>
+  <si>
+    <t>Post 3</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>fys1</t>
+  </si>
+  <si>
+    <t>mat3</t>
+  </si>
+  <si>
+    <t>nano</t>
+  </si>
+  <si>
+    <t>Post 4</t>
+  </si>
+  <si>
+    <t>dat4</t>
+  </si>
+  <si>
+    <t>dat7</t>
+  </si>
+  <si>
+    <t>hold2</t>
+  </si>
+  <si>
+    <t>mat1</t>
+  </si>
+  <si>
+    <t>Post 5</t>
+  </si>
+  <si>
+    <t>dat2</t>
+  </si>
+  <si>
     <t>hold1</t>
   </si>
   <si>
+    <t>it1</t>
+  </si>
+  <si>
     <t>møk2</t>
   </si>
   <si>
-    <t>TK</t>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>dat5</t>
+  </si>
+  <si>
+    <t>dat6</t>
   </si>
   <si>
     <t>fys5</t>
   </si>
   <si>
-    <t>Post 2</t>
-  </si>
-  <si>
-    <t>fys4</t>
-  </si>
-  <si>
-    <t>hold2</t>
-  </si>
-  <si>
-    <t>dat5</t>
-  </si>
-  <si>
-    <t>fys2</t>
-  </si>
-  <si>
-    <t>Post 3</t>
-  </si>
-  <si>
-    <t>mat2</t>
-  </si>
-  <si>
     <t>møk1</t>
-  </si>
-  <si>
-    <t>dat3</t>
-  </si>
-  <si>
-    <t>dat1</t>
-  </si>
-  <si>
-    <t>Post 4</t>
-  </si>
-  <si>
-    <t>dat6</t>
-  </si>
-  <si>
-    <t>dat7</t>
-  </si>
-  <si>
-    <t>dat4</t>
-  </si>
-  <si>
-    <t>fys1</t>
-  </si>
-  <si>
-    <t>Post 5</t>
-  </si>
-  <si>
-    <t>nano</t>
-  </si>
-  <si>
-    <t>dav</t>
-  </si>
-  <si>
-    <t>mat3</t>
-  </si>
-  <si>
-    <t>it1</t>
-  </si>
-  <si>
-    <t>Pause</t>
-  </si>
-  <si>
-    <t>mat1</t>
-  </si>
-  <si>
-    <t>dat2</t>
-  </si>
-  <si>
-    <t>it2</t>
-  </si>
-  <si>
-    <t>fys3</t>
   </si>
   <si>
     <t>14:35-14:45</t>
@@ -620,16 +620,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -637,16 +637,16 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -654,16 +654,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -671,16 +671,16 @@
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -688,16 +688,16 @@
         <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -705,13 +705,13 @@
         <v>26</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>25</v>
@@ -731,16 +731,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E20" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -748,16 +748,16 @@
         <v>6</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -765,16 +765,16 @@
         <v>11</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -782,16 +782,16 @@
         <v>16</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -799,16 +799,16 @@
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -816,7 +816,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>13</v>
@@ -825,7 +825,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" customHeight="1">
@@ -842,16 +842,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -859,16 +859,16 @@
         <v>6</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -876,16 +876,16 @@
         <v>11</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -893,16 +893,16 @@
         <v>16</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="E32" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -910,16 +910,16 @@
         <v>21</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -953,16 +953,16 @@
         <v>1</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -970,16 +970,16 @@
         <v>6</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -987,16 +987,16 @@
         <v>11</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1004,16 +1004,16 @@
         <v>16</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1021,13 +1021,13 @@
         <v>21</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>30</v>
@@ -1038,16 +1038,16 @@
         <v>26</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" customHeight="1">
@@ -1064,16 +1064,16 @@
         <v>1</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1081,16 +1081,16 @@
         <v>6</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1098,16 +1098,16 @@
         <v>11</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D49" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1115,16 +1115,16 @@
         <v>16</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1132,16 +1132,16 @@
         <v>21</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:5">

</xml_diff>